<commit_message>
Expanding the Itto class and the DamageEngine class. Ran into an issue with importing modules. test.py throws an error when importing itto class as that class can't find the Functions module when being run from the test class. Works when run from Itto class.
</commit_message>
<xml_diff>
--- a/Characters/DataTables/IttoTables.xlsx
+++ b/Characters/DataTables/IttoTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Documents\GenshinCoding\GenshinIndex\Characters\DataTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC25FEB-2DA2-4BE7-90AE-5C9561E214E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44946CB7-0BFD-448C-8C42-2CAA4DE1A642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="121">
   <si>
     <t>1_Hit</t>
   </si>
@@ -385,6 +385,9 @@
   </si>
   <si>
     <t>EHoldCD</t>
+  </si>
+  <si>
+    <t>Dash</t>
   </si>
 </sst>
 </file>
@@ -745,7 +748,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -846,6 +849,14 @@
     </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1384,10 +1395,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2057,6 +2068,56 @@
       </c>
       <c r="Q13" s="33"/>
     </row>
+    <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="40">
+        <v>0</v>
+      </c>
+      <c r="C14" s="40">
+        <v>0</v>
+      </c>
+      <c r="D14" s="40">
+        <v>0</v>
+      </c>
+      <c r="E14" s="40">
+        <v>0</v>
+      </c>
+      <c r="F14" s="40">
+        <v>0</v>
+      </c>
+      <c r="G14" s="40">
+        <v>0</v>
+      </c>
+      <c r="H14" s="40">
+        <v>0</v>
+      </c>
+      <c r="I14" s="40">
+        <v>0</v>
+      </c>
+      <c r="J14" s="40">
+        <v>0</v>
+      </c>
+      <c r="K14" s="40">
+        <v>0</v>
+      </c>
+      <c r="L14" s="40">
+        <v>0</v>
+      </c>
+      <c r="M14" s="40">
+        <v>0</v>
+      </c>
+      <c r="N14" s="40">
+        <v>0</v>
+      </c>
+      <c r="O14" s="40">
+        <v>0</v>
+      </c>
+      <c r="P14" s="40">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2067,10 +2128,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2324,6 +2385,24 @@
       <c r="P5" s="2">
         <v>10</v>
       </c>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="37"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2337,7 +2416,9 @@
   </sheetPr>
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>